<commit_message>
feat: strong update MID folder
</commit_message>
<xml_diff>
--- a/04 - MID/01 - Create/01 - InstallLocation/Data.xlsx
+++ b/04 - MID/01 - Create/01 - InstallLocation/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\MID\Create-InstallLocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mao8ct\Desktop\PyAutomateSAP\04 - MID\01 - Create\01 - InstallLocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D47BA3-F870-4044-A26A-8E5FFAA0E81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8B7DE8-CB74-4D3A-AF9A-01CED784BC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{841C4129-0CB3-4066-B34E-E8845E3509BE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Norma</t>
   </si>
@@ -44,16 +44,7 @@
     <t>Quantidade</t>
   </si>
   <si>
-    <t xml:space="preserve">4729108508 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4328700313 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4729106784 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4729107242 </t>
+    <t>MAGAZINE MIKRON</t>
   </si>
 </sst>
 </file>
@@ -121,12 +112,12 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -147,9 +138,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +178,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -293,7 +284,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,7 +426,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -445,64 +436,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D997F1F-30FE-4A2A-B694-A9178A4FC344}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>8</v>
+      <c r="B2" s="3">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>41</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>54</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>54</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A5" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>